<commit_message>
Josefines Stuff - Pairs, Triples, etc
</commit_message>
<xml_diff>
--- a/Evaluation.xlsx
+++ b/Evaluation.xlsx
@@ -9,30 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation" sheetId="1" r:id="rId1"/>
     <sheet name="All Ratings" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Evaluation!$A$2:$A$11</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Evaluation!$B$2:$B$37</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Evaluation!$F$2:$F$37</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'All Ratings'!$B$2:$B$181</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'All Ratings'!$B$2:$B$181</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'All Ratings'!$A$2:$A$181</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Evaluation!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Evaluation!$D$2:$D$37</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Evaluation!$E$2:$E$37</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Evaluation!$F$2:$F$37</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Evaluation!$B$2:$B$37</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Evaluation!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Evaluation!$D$2:$D$37</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Evaluation!$E$2:$E$37</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Evaluation!$S$2:$S$37</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Evaluation!$T$2:$T$37</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Evaluation!$V$2:$V$37</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Evaluation!$S$2:$S$37</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'All Ratings'!$B$2:$B$181</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'All Ratings'!$A$2:$A$181</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -158,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -166,6 +157,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,7 +180,43 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{3EC4EE99-6542-4E74-80ED-57BBBC4A31CC}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binCount val="11"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -247,12 +275,12 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -390,6 +418,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -1406,7 +1474,598 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA876446-58D1-46D8-B804-349A7A47ED0C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2667000" y="1047750"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-DE" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1455,8 +2114,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2627779" y="318245"/>
-              <a:ext cx="5197288" cy="3390900"/>
+              <a:off x="2600885" y="312642"/>
+              <a:ext cx="5143500" cy="3295650"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1533,8 +2192,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2872657" y="4607026"/>
-              <a:ext cx="4531775" cy="2733144"/>
+              <a:off x="2868749" y="4494680"/>
+              <a:ext cx="4523960" cy="2664759"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1864,10 +2523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2:V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,7 +2538,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +2591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1990,9 +2649,24 @@
         <f>IF(O2&gt;=6,1,0)</f>
         <v>0</v>
       </c>
-      <c r="S2" s="3"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S2" s="3">
+        <f>IF(N2&gt;=5,MAX(B2:F2),MIN(B2:F2))</f>
+        <v>1</v>
+      </c>
+      <c r="T2" s="7">
+        <f>IF(N2&gt;=5,AVERAGE(LARGE(B2:F2,{1;2;3})),AVERAGE(LARGE(B2:F2,{3;4;5})))</f>
+        <v>2</v>
+      </c>
+      <c r="U2" s="1">
+        <f>VAR(B2:F2)</f>
+        <v>9.5</v>
+      </c>
+      <c r="V2" s="1">
+        <f>IF(N2&gt;=5,AVERAGE(LARGE(B2:F2,{1;2;3;4})),AVERAGE(LARGE(B2:F2,{2;3;4;5})))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2050,9 +2724,24 @@
         <f t="shared" ref="R3:R37" si="5">IF(O3&gt;=6,1,0)</f>
         <v>0</v>
       </c>
-      <c r="S3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S3" s="3">
+        <f t="shared" ref="S3:S37" si="6">IF(N3&gt;=5,MAX(B3:F3),MIN(B3:F3))</f>
+        <v>8</v>
+      </c>
+      <c r="T3" s="7">
+        <f>IF(N3&gt;=5,AVERAGE(LARGE(B3:F3,{1;2;3})),AVERAGE(LARGE(B3:F3,{3;4;5})))</f>
+        <v>7</v>
+      </c>
+      <c r="U3" s="1">
+        <f t="shared" ref="U3:U37" si="7">VAR(B3:F3)</f>
+        <v>5.7999999999999972</v>
+      </c>
+      <c r="V3" s="1">
+        <f>IF(N3&gt;=5,AVERAGE(LARGE(B3:F3,{1;2;3;4})),AVERAGE(LARGE(B3:F3,{2;3;4;5})))</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2110,9 +2799,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S4" s="3"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S4" s="3">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="T4" s="7">
+        <f>IF(N4&gt;=5,AVERAGE(LARGE(B4:F4,{1;2;3})),AVERAGE(LARGE(B4:F4,{3;4;5})))</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="U4" s="1">
+        <f t="shared" si="7"/>
+        <v>9.2000000000000028</v>
+      </c>
+      <c r="V4" s="1">
+        <f>IF(N4&gt;=5,AVERAGE(LARGE(B4:F4,{1;2;3;4})),AVERAGE(LARGE(B4:F4,{2;3;4;5})))</f>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2170,9 +2874,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S5" s="3"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S5" s="3">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="T5" s="7">
+        <f>IF(N5&gt;=5,AVERAGE(LARGE(B5:F5,{1;2;3})),AVERAGE(LARGE(B5:F5,{3;4;5})))</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" si="7"/>
+        <v>1.2000000000000028</v>
+      </c>
+      <c r="V5" s="1">
+        <f>IF(N5&gt;=5,AVERAGE(LARGE(B5:F5,{1;2;3;4})),AVERAGE(LARGE(B5:F5,{2;3;4;5})))</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2230,9 +2949,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S6" s="3"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S6" s="3">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="T6" s="7">
+        <f>IF(N6&gt;=5,AVERAGE(LARGE(B6:F6,{1;2;3})),AVERAGE(LARGE(B6:F6,{3;4;5})))</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="U6" s="1">
+        <f t="shared" si="7"/>
+        <v>0.69999999999999929</v>
+      </c>
+      <c r="V6" s="1">
+        <f>IF(N6&gt;=5,AVERAGE(LARGE(B6:F6,{1;2;3;4})),AVERAGE(LARGE(B6:F6,{2;3;4;5})))</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2290,9 +3024,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S7" s="3"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S7" s="3">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="T7" s="7">
+        <f>IF(N7&gt;=5,AVERAGE(LARGE(B7:F7,{1;2;3})),AVERAGE(LARGE(B7:F7,{3;4;5})))</f>
+        <v>7</v>
+      </c>
+      <c r="U7" s="1">
+        <f t="shared" si="7"/>
+        <v>9.2999999999999972</v>
+      </c>
+      <c r="V7" s="1">
+        <f>IF(N7&gt;=5,AVERAGE(LARGE(B7:F7,{1;2;3;4})),AVERAGE(LARGE(B7:F7,{2;3;4;5})))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2350,9 +3099,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S8" s="3"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S8" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T8" s="7">
+        <f>IF(N8&gt;=5,AVERAGE(LARGE(B8:F8,{1;2;3})),AVERAGE(LARGE(B8:F8,{3;4;5})))</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="7"/>
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="V8" s="1">
+        <f>IF(N8&gt;=5,AVERAGE(LARGE(B8:F8,{1;2;3;4})),AVERAGE(LARGE(B8:F8,{2;3;4;5})))</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2410,9 +3174,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S9" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T9" s="7">
+        <f>IF(N9&gt;=5,AVERAGE(LARGE(B9:F9,{1;2;3})),AVERAGE(LARGE(B9:F9,{3;4;5})))</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="U9" s="1">
+        <f t="shared" si="7"/>
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="V9" s="1">
+        <f>IF(N9&gt;=5,AVERAGE(LARGE(B9:F9,{1;2;3;4})),AVERAGE(LARGE(B9:F9,{2;3;4;5})))</f>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2470,9 +3249,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S10" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T10" s="7">
+        <f>IF(N10&gt;=5,AVERAGE(LARGE(B10:F10,{1;2;3})),AVERAGE(LARGE(B10:F10,{3;4;5})))</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="U10" s="1">
+        <f t="shared" si="7"/>
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="V10" s="1">
+        <f>IF(N10&gt;=5,AVERAGE(LARGE(B10:F10,{1;2;3;4})),AVERAGE(LARGE(B10:F10,{2;3;4;5})))</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2530,9 +3324,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S11" s="3"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S11" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="7">
+        <f>IF(N11&gt;=5,AVERAGE(LARGE(B11:F11,{1;2;3})),AVERAGE(LARGE(B11:F11,{3;4;5})))</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="U11" s="1">
+        <f t="shared" si="7"/>
+        <v>11.3</v>
+      </c>
+      <c r="V11" s="1">
+        <f>IF(N11&gt;=5,AVERAGE(LARGE(B11:F11,{1;2;3;4})),AVERAGE(LARGE(B11:F11,{2;3;4;5})))</f>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2590,9 +3399,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S12" s="3"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S12" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="T12" s="7">
+        <f>IF(N12&gt;=5,AVERAGE(LARGE(B12:F12,{1;2;3})),AVERAGE(LARGE(B12:F12,{3;4;5})))</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="U12" s="1">
+        <f t="shared" si="7"/>
+        <v>3.3000000000000007</v>
+      </c>
+      <c r="V12" s="1">
+        <f>IF(N12&gt;=5,AVERAGE(LARGE(B12:F12,{1;2;3;4})),AVERAGE(LARGE(B12:F12,{2;3;4;5})))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2650,9 +3474,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S13" s="3"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S13" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="T13" s="7">
+        <f>IF(N13&gt;=5,AVERAGE(LARGE(B13:F13,{1;2;3})),AVERAGE(LARGE(B13:F13,{3;4;5})))</f>
+        <v>3</v>
+      </c>
+      <c r="U13" s="1">
+        <f t="shared" si="7"/>
+        <v>5.3000000000000007</v>
+      </c>
+      <c r="V13" s="1">
+        <f>IF(N13&gt;=5,AVERAGE(LARGE(B13:F13,{1;2;3;4})),AVERAGE(LARGE(B13:F13,{2;3;4;5})))</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2710,9 +3549,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S14" s="3"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S14" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="T14" s="7">
+        <f>IF(N14&gt;=5,AVERAGE(LARGE(B14:F14,{1;2;3})),AVERAGE(LARGE(B14:F14,{3;4;5})))</f>
+        <v>4</v>
+      </c>
+      <c r="U14" s="1">
+        <f t="shared" si="7"/>
+        <v>2.6999999999999993</v>
+      </c>
+      <c r="V14" s="1">
+        <f>IF(N14&gt;=5,AVERAGE(LARGE(B14:F14,{1;2;3;4})),AVERAGE(LARGE(B14:F14,{2;3;4;5})))</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2770,9 +3624,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S15" s="3"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S15" s="3">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="T15" s="7">
+        <f>IF(N15&gt;=5,AVERAGE(LARGE(B15:F15,{1;2;3})),AVERAGE(LARGE(B15:F15,{3;4;5})))</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U15" s="1">
+        <f t="shared" si="7"/>
+        <v>1.7000000000000028</v>
+      </c>
+      <c r="V15" s="1">
+        <f>IF(N15&gt;=5,AVERAGE(LARGE(B15:F15,{1;2;3;4})),AVERAGE(LARGE(B15:F15,{2;3;4;5})))</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2830,9 +3699,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S16" s="3"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S16" s="3">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="T16" s="7">
+        <f>IF(N16&gt;=5,AVERAGE(LARGE(B16:F16,{1;2;3})),AVERAGE(LARGE(B16:F16,{3;4;5})))</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U16" s="1">
+        <f t="shared" si="7"/>
+        <v>3.7999999999999972</v>
+      </c>
+      <c r="V16" s="1">
+        <f>IF(N16&gt;=5,AVERAGE(LARGE(B16:F16,{1;2;3;4})),AVERAGE(LARGE(B16:F16,{2;3;4;5})))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2890,9 +3774,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S17" s="3"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S17" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T17" s="7">
+        <f>IF(N17&gt;=5,AVERAGE(LARGE(B17:F17,{1;2;3})),AVERAGE(LARGE(B17:F17,{3;4;5})))</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="U17" s="1">
+        <f t="shared" si="7"/>
+        <v>13.3</v>
+      </c>
+      <c r="V17" s="1">
+        <f>IF(N17&gt;=5,AVERAGE(LARGE(B17:F17,{1;2;3;4})),AVERAGE(LARGE(B17:F17,{2;3;4;5})))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2950,9 +3849,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S18" s="3"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S18" s="3">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="T18" s="7">
+        <f>IF(N18&gt;=5,AVERAGE(LARGE(B18:F18,{1;2;3})),AVERAGE(LARGE(B18:F18,{3;4;5})))</f>
+        <v>8</v>
+      </c>
+      <c r="U18" s="1">
+        <f t="shared" si="7"/>
+        <v>3.7000000000000028</v>
+      </c>
+      <c r="V18" s="1">
+        <f>IF(N18&gt;=5,AVERAGE(LARGE(B18:F18,{1;2;3;4})),AVERAGE(LARGE(B18:F18,{2;3;4;5})))</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3010,9 +3924,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S19" s="3"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S19" s="3">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="T19" s="7">
+        <f>IF(N19&gt;=5,AVERAGE(LARGE(B19:F19,{1;2;3})),AVERAGE(LARGE(B19:F19,{3;4;5})))</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U19" s="1">
+        <f t="shared" si="7"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="V19" s="1">
+        <f>IF(N19&gt;=5,AVERAGE(LARGE(B19:F19,{1;2;3;4})),AVERAGE(LARGE(B19:F19,{2;3;4;5})))</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3070,9 +3999,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S20" s="3"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S20" s="3">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="T20" s="7">
+        <f>IF(N20&gt;=5,AVERAGE(LARGE(B20:F20,{1;2;3})),AVERAGE(LARGE(B20:F20,{3;4;5})))</f>
+        <v>7</v>
+      </c>
+      <c r="U20" s="1">
+        <f t="shared" si="7"/>
+        <v>9.7000000000000028</v>
+      </c>
+      <c r="V20" s="1">
+        <f>IF(N20&gt;=5,AVERAGE(LARGE(B20:F20,{1;2;3;4})),AVERAGE(LARGE(B20:F20,{2;3;4;5})))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3130,9 +4074,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S21" s="3"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S21" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="T21" s="7">
+        <f>IF(N21&gt;=5,AVERAGE(LARGE(B21:F21,{1;2;3})),AVERAGE(LARGE(B21:F21,{3;4;5})))</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="U21" s="1">
+        <f t="shared" si="7"/>
+        <v>4.6999999999999993</v>
+      </c>
+      <c r="V21" s="1">
+        <f>IF(N21&gt;=5,AVERAGE(LARGE(B21:F21,{1;2;3;4})),AVERAGE(LARGE(B21:F21,{2;3;4;5})))</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3191,9 +4150,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S22" s="3"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S22" s="3">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="T22" s="7">
+        <f>IF(N22&gt;=5,AVERAGE(LARGE(B22:F22,{1;2;3})),AVERAGE(LARGE(B22:F22,{3;4;5})))</f>
+        <v>7</v>
+      </c>
+      <c r="U22" s="1">
+        <f t="shared" si="7"/>
+        <v>7.2999999999999972</v>
+      </c>
+      <c r="V22" s="1">
+        <f>IF(N22&gt;=5,AVERAGE(LARGE(B22:F22,{1;2;3;4})),AVERAGE(LARGE(B22:F22,{2;3;4;5})))</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3251,9 +4225,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S23" s="3"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S23" s="3">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="T23" s="7">
+        <f>IF(N23&gt;=5,AVERAGE(LARGE(B23:F23,{1;2;3})),AVERAGE(LARGE(B23:F23,{3;4;5})))</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U23" s="1">
+        <f t="shared" si="7"/>
+        <v>1.7000000000000028</v>
+      </c>
+      <c r="V23" s="1">
+        <f>IF(N23&gt;=5,AVERAGE(LARGE(B23:F23,{1;2;3;4})),AVERAGE(LARGE(B23:F23,{2;3;4;5})))</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3311,9 +4300,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S24" s="3"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S24" s="3">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="T24" s="7">
+        <f>IF(N24&gt;=5,AVERAGE(LARGE(B24:F24,{1;2;3})),AVERAGE(LARGE(B24:F24,{3;4;5})))</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="U24" s="1">
+        <f t="shared" si="7"/>
+        <v>3.3000000000000007</v>
+      </c>
+      <c r="V24" s="1">
+        <f>IF(N24&gt;=5,AVERAGE(LARGE(B24:F24,{1;2;3;4})),AVERAGE(LARGE(B24:F24,{2;3;4;5})))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3371,9 +4375,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S25" s="3"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S25" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="T25" s="7">
+        <f>IF(N25&gt;=5,AVERAGE(LARGE(B25:F25,{1;2;3})),AVERAGE(LARGE(B25:F25,{3;4;5})))</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="U25" s="1">
+        <f t="shared" si="7"/>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="V25" s="1">
+        <f>IF(N25&gt;=5,AVERAGE(LARGE(B25:F25,{1;2;3;4})),AVERAGE(LARGE(B25:F25,{2;3;4;5})))</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3431,9 +4450,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S26" s="3"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S26" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T26" s="7">
+        <f>IF(N26&gt;=5,AVERAGE(LARGE(B26:F26,{1;2;3})),AVERAGE(LARGE(B26:F26,{3;4;5})))</f>
+        <v>3</v>
+      </c>
+      <c r="U26" s="1">
+        <f t="shared" si="7"/>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="V26" s="1">
+        <f>IF(N26&gt;=5,AVERAGE(LARGE(B26:F26,{1;2;3;4})),AVERAGE(LARGE(B26:F26,{2;3;4;5})))</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3491,9 +4525,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S27" s="3"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S27" s="3">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="T27" s="7">
+        <f>IF(N27&gt;=5,AVERAGE(LARGE(B27:F27,{1;2;3})),AVERAGE(LARGE(B27:F27,{3;4;5})))</f>
+        <v>9</v>
+      </c>
+      <c r="U27" s="1">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="V27" s="1">
+        <f>IF(N27&gt;=5,AVERAGE(LARGE(B27:F27,{1;2;3;4})),AVERAGE(LARGE(B27:F27,{2;3;4;5})))</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3551,9 +4600,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S28" s="3"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S28" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T28" s="7">
+        <f>IF(N28&gt;=5,AVERAGE(LARGE(B28:F28,{1;2;3})),AVERAGE(LARGE(B28:F28,{3;4;5})))</f>
+        <v>3</v>
+      </c>
+      <c r="U28" s="1">
+        <f t="shared" si="7"/>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="V28" s="1">
+        <f>IF(N28&gt;=5,AVERAGE(LARGE(B28:F28,{1;2;3;4})),AVERAGE(LARGE(B28:F28,{2;3;4;5})))</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3611,9 +4675,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S29" s="3"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S29" s="3">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="T29" s="7">
+        <f>IF(N29&gt;=5,AVERAGE(LARGE(B29:F29,{1;2;3})),AVERAGE(LARGE(B29:F29,{3;4;5})))</f>
+        <v>7</v>
+      </c>
+      <c r="U29" s="1">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="V29" s="1">
+        <f>IF(N29&gt;=5,AVERAGE(LARGE(B29:F29,{1;2;3;4})),AVERAGE(LARGE(B29:F29,{2;3;4;5})))</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3671,9 +4750,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S30" s="3"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S30" s="3">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="T30" s="7">
+        <f>IF(N30&gt;=5,AVERAGE(LARGE(B30:F30,{1;2;3})),AVERAGE(LARGE(B30:F30,{3;4;5})))</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="U30" s="1">
+        <f t="shared" si="7"/>
+        <v>17.299999999999997</v>
+      </c>
+      <c r="V30" s="1">
+        <f>IF(N30&gt;=5,AVERAGE(LARGE(B30:F30,{1;2;3;4})),AVERAGE(LARGE(B30:F30,{2;3;4;5})))</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3731,9 +4825,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S31" s="3"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S31" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T31" s="7">
+        <f>IF(N31&gt;=5,AVERAGE(LARGE(B31:F31,{1;2;3})),AVERAGE(LARGE(B31:F31,{3;4;5})))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="U31" s="1">
+        <f t="shared" si="7"/>
+        <v>2.8</v>
+      </c>
+      <c r="V31" s="1">
+        <f>IF(N31&gt;=5,AVERAGE(LARGE(B31:F31,{1;2;3;4})),AVERAGE(LARGE(B31:F31,{2;3;4;5})))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3791,9 +4900,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S32" s="3"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S32" s="3">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="T32" s="7">
+        <f>IF(N32&gt;=5,AVERAGE(LARGE(B32:F32,{1;2;3})),AVERAGE(LARGE(B32:F32,{3;4;5})))</f>
+        <v>7</v>
+      </c>
+      <c r="U32" s="1">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="V32" s="1">
+        <f>IF(N32&gt;=5,AVERAGE(LARGE(B32:F32,{1;2;3;4})),AVERAGE(LARGE(B32:F32,{2;3;4;5})))</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3851,9 +4975,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S33" s="3"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S33" s="3">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="T33" s="7">
+        <f>IF(N33&gt;=5,AVERAGE(LARGE(B33:F33,{1;2;3})),AVERAGE(LARGE(B33:F33,{3;4;5})))</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="U33" s="1">
+        <f t="shared" si="7"/>
+        <v>6.3000000000000007</v>
+      </c>
+      <c r="V33" s="1">
+        <f>IF(N33&gt;=5,AVERAGE(LARGE(B33:F33,{1;2;3;4})),AVERAGE(LARGE(B33:F33,{2;3;4;5})))</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3911,9 +5050,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S34" s="3"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S34" s="3">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="T34" s="7">
+        <f>IF(N34&gt;=5,AVERAGE(LARGE(B34:F34,{1;2;3})),AVERAGE(LARGE(B34:F34,{3;4;5})))</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="U34" s="1">
+        <f t="shared" si="7"/>
+        <v>9.7999999999999972</v>
+      </c>
+      <c r="V34" s="1">
+        <f>IF(N34&gt;=5,AVERAGE(LARGE(B34:F34,{1;2;3;4})),AVERAGE(LARGE(B34:F34,{2;3;4;5})))</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3971,9 +5125,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S35" s="3"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S35" s="3">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="T35" s="7">
+        <f>IF(N35&gt;=5,AVERAGE(LARGE(B35:F35,{1;2;3})),AVERAGE(LARGE(B35:F35,{3;4;5})))</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="U35" s="1">
+        <f t="shared" si="7"/>
+        <v>1.2000000000000028</v>
+      </c>
+      <c r="V35" s="1">
+        <f>IF(N35&gt;=5,AVERAGE(LARGE(B35:F35,{1;2;3;4})),AVERAGE(LARGE(B35:F35,{2;3;4;5})))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -4031,9 +5200,24 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="S36" s="3"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S36" s="3">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="T36" s="7">
+        <f>IF(N36&gt;=5,AVERAGE(LARGE(B36:F36,{1;2;3})),AVERAGE(LARGE(B36:F36,{3;4;5})))</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="U36" s="1">
+        <f t="shared" si="7"/>
+        <v>3.7000000000000028</v>
+      </c>
+      <c r="V36" s="1">
+        <f>IF(N36&gt;=5,AVERAGE(LARGE(B36:F36,{1;2;3;4})),AVERAGE(LARGE(B36:F36,{2;3;4;5})))</f>
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -4091,7 +5275,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S37" s="3"/>
+      <c r="S37" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="T37" s="7">
+        <f>IF(N37&gt;=5,AVERAGE(LARGE(B37:F37,{1;2;3})),AVERAGE(LARGE(B37:F37,{3;4;5})))</f>
+        <v>3</v>
+      </c>
+      <c r="U37" s="1">
+        <f t="shared" si="7"/>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="V37" s="1">
+        <f>IF(N37&gt;=5,AVERAGE(LARGE(B37:F37,{1;2;3;4})),AVERAGE(LARGE(B37:F37,{2;3;4;5})))</f>
+        <v>3.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4099,6 +5298,7 @@
   <ignoredErrors>
     <ignoredError sqref="M2" formulaRange="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Renaming Target Variables, correcting Typo
</commit_message>
<xml_diff>
--- a/Evaluation.xlsx
+++ b/Evaluation.xlsx
@@ -9,19 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation" sheetId="1" r:id="rId1"/>
     <sheet name="All Ratings" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Evaluation!$S$2:$S$37</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Evaluation!$T$2:$T$37</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Evaluation!$V$2:$V$37</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Evaluation!$S$2:$S$37</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'All Ratings'!$B$2:$B$181</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'All Ratings'!$A$2:$A$181</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Evaluation!$V$2:$V$37</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'All Ratings'!$B$2:$B$181</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'All Ratings'!$A$2:$A$181</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -68,28 +65,40 @@
     <t>Recom 5</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t>Rounded Average</t>
-  </si>
-  <si>
-    <t>Average Recom</t>
-  </si>
-  <si>
-    <t>Avg &gt;=6</t>
-  </si>
-  <si>
-    <t>Med &gt;=6</t>
-  </si>
-  <si>
     <t>All Tastes</t>
   </si>
   <si>
     <t>All Recom</t>
+  </si>
+  <si>
+    <t>Med_Rating</t>
+  </si>
+  <si>
+    <t>Avg_Rating</t>
+  </si>
+  <si>
+    <t>Avg_Rating_Rounded</t>
+  </si>
+  <si>
+    <t>Recommondation</t>
+  </si>
+  <si>
+    <t>Dummy_Avg</t>
+  </si>
+  <si>
+    <t>Dummy_Median</t>
+  </si>
+  <si>
+    <t>Polarised_Rating</t>
+  </si>
+  <si>
+    <t>Polarised_Rating2</t>
+  </si>
+  <si>
+    <t>Polarised_Rating3</t>
+  </si>
+  <si>
+    <t>Variance_Rating</t>
   </si>
 </sst>
 </file>
@@ -180,7 +189,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -216,7 +225,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -280,7 +289,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2525,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V37"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,22 +2582,34 @@
         <v>10</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -5317,10 +5338,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>